<commit_message>
added lookup methods to fill address name from address_name table based on degree and minute
</commit_message>
<xml_diff>
--- a/Seed_Table_for_Address_Names.xlsx
+++ b/Seed_Table_for_Address_Names.xlsx
@@ -2,12 +2,12 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="16460" yWindow="0" windowWidth="8060" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Seed_Table" sheetId="1" r:id="rId1"/>
+    <sheet name="Seed_Table_for_Address_Names.cs" sheetId="1" r:id="rId1"/>
     <sheet name="consanants_first" sheetId="2" r:id="rId2"/>
     <sheet name="vowels_first" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -6887,7 +6887,7 @@
     <t>iza</t>
   </si>
   <si>
-    <t>*used first 60 entries from vowels_first and then consants_first 'b','t',and 'n' trailing letter columns for 61-360</t>
+    <t>origin</t>
   </si>
 </sst>
 </file>
@@ -6971,13 +6971,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="33">
@@ -7342,3096 +7339,3132 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E364"/>
+  <dimension ref="A1:D370"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView tabSelected="1" topLeftCell="A344" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B371" sqref="B371"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5">
-      <c r="E2" s="2" t="s">
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2288</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="1" t="s">
+    <row r="3" spans="1:4">
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>2228</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
       <c r="D4" s="1" t="s">
+        <v>2229</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="B5">
-        <v>1</v>
-      </c>
       <c r="C5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>2228</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>2230</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="B6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>2229</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>2231</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="B7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>2230</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>2232</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="B8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C8">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>2231</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>2233</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="B9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>2232</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>2234</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="B10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C10">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>2233</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>2235</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="B11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C11">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>2234</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="B12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>2235</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
+        <v>2237</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="B13">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C13">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>2236</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+        <v>2238</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="B14">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>2237</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
+        <v>2239</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="B15">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C15">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>2238</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="B16">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C16">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2239</v>
+        <v>2241</v>
       </c>
     </row>
     <row r="17" spans="2:4">
       <c r="B17">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C17">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>2240</v>
+        <v>2242</v>
       </c>
     </row>
     <row r="18" spans="2:4">
       <c r="B18">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C18">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>2241</v>
+        <v>2243</v>
       </c>
     </row>
     <row r="19" spans="2:4">
       <c r="B19">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>2242</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="20" spans="2:4">
       <c r="B20">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>2243</v>
+        <v>2245</v>
       </c>
     </row>
     <row r="21" spans="2:4">
       <c r="B21">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C21">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>2244</v>
+        <v>2246</v>
       </c>
     </row>
     <row r="22" spans="2:4">
       <c r="B22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C22">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>2245</v>
+        <v>2247</v>
       </c>
     </row>
     <row r="23" spans="2:4">
       <c r="B23">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>2246</v>
+        <v>2248</v>
       </c>
     </row>
     <row r="24" spans="2:4">
       <c r="B24">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>2247</v>
+        <v>2249</v>
       </c>
     </row>
     <row r="25" spans="2:4">
       <c r="B25">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C25">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>2248</v>
+        <v>2250</v>
       </c>
     </row>
     <row r="26" spans="2:4">
       <c r="B26">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C26">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>2249</v>
+        <v>2251</v>
       </c>
     </row>
     <row r="27" spans="2:4">
       <c r="B27">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C27">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>2250</v>
+        <v>2252</v>
       </c>
     </row>
     <row r="28" spans="2:4">
       <c r="B28">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C28">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>2251</v>
+        <v>2253</v>
       </c>
     </row>
     <row r="29" spans="2:4">
       <c r="B29">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C29">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>2252</v>
+        <v>2254</v>
       </c>
     </row>
     <row r="30" spans="2:4">
       <c r="B30">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C30">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>2253</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="31" spans="2:4">
       <c r="B31">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C31">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>2254</v>
+        <v>2256</v>
       </c>
     </row>
     <row r="32" spans="2:4">
       <c r="B32">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C32">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>2255</v>
+        <v>2257</v>
       </c>
     </row>
     <row r="33" spans="2:4">
       <c r="B33">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C33">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>2256</v>
+        <v>2258</v>
       </c>
     </row>
     <row r="34" spans="2:4">
       <c r="B34">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C34">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>2257</v>
+        <v>2259</v>
       </c>
     </row>
     <row r="35" spans="2:4">
       <c r="B35">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C35">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>2258</v>
+        <v>2260</v>
       </c>
     </row>
     <row r="36" spans="2:4">
       <c r="B36">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C36">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>2259</v>
+        <v>2261</v>
       </c>
     </row>
     <row r="37" spans="2:4">
       <c r="B37">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C37">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>2260</v>
+        <v>2262</v>
       </c>
     </row>
     <row r="38" spans="2:4">
       <c r="B38">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C38">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>2261</v>
+        <v>2263</v>
       </c>
     </row>
     <row r="39" spans="2:4">
       <c r="B39">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C39">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>2262</v>
+        <v>2264</v>
       </c>
     </row>
     <row r="40" spans="2:4">
       <c r="B40">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C40">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>2263</v>
+        <v>2265</v>
       </c>
     </row>
     <row r="41" spans="2:4">
       <c r="B41">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C41">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>2264</v>
+        <v>2266</v>
       </c>
     </row>
     <row r="42" spans="2:4">
       <c r="B42">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C42">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>2265</v>
+        <v>2267</v>
       </c>
     </row>
     <row r="43" spans="2:4">
       <c r="B43">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C43">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>2266</v>
+        <v>2268</v>
       </c>
     </row>
     <row r="44" spans="2:4">
       <c r="B44">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C44">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>2267</v>
+        <v>2269</v>
       </c>
     </row>
     <row r="45" spans="2:4">
       <c r="B45">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C45">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>2268</v>
+        <v>2270</v>
       </c>
     </row>
     <row r="46" spans="2:4">
       <c r="B46">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C46">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>2269</v>
+        <v>2271</v>
       </c>
     </row>
     <row r="47" spans="2:4">
       <c r="B47">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C47">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>2270</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="48" spans="2:4">
       <c r="B48">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C48">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>2271</v>
+        <v>2273</v>
       </c>
     </row>
     <row r="49" spans="2:4">
       <c r="B49">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C49">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>2272</v>
+        <v>2274</v>
       </c>
     </row>
     <row r="50" spans="2:4">
       <c r="B50">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C50">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>2273</v>
+        <v>2275</v>
       </c>
     </row>
     <row r="51" spans="2:4">
       <c r="B51">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C51">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>2274</v>
+        <v>2276</v>
       </c>
     </row>
     <row r="52" spans="2:4">
       <c r="B52">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C52">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>2275</v>
+        <v>2277</v>
       </c>
     </row>
     <row r="53" spans="2:4">
       <c r="B53">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C53">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>2276</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="54" spans="2:4">
       <c r="B54">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C54">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>2277</v>
+        <v>2279</v>
       </c>
     </row>
     <row r="55" spans="2:4">
       <c r="B55">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C55">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>2278</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="56" spans="2:4">
       <c r="B56">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C56">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>2279</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="57" spans="2:4">
       <c r="B57">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C57">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>2280</v>
+        <v>2282</v>
       </c>
     </row>
     <row r="58" spans="2:4">
       <c r="B58">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C58">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>2281</v>
+        <v>2283</v>
       </c>
     </row>
     <row r="59" spans="2:4">
       <c r="B59">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C59">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>2282</v>
+        <v>2284</v>
       </c>
     </row>
     <row r="60" spans="2:4">
       <c r="B60">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C60">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>2283</v>
+        <v>2285</v>
       </c>
     </row>
     <row r="61" spans="2:4">
       <c r="B61">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C61">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>2284</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="62" spans="2:4">
       <c r="B62">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C62">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>2285</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="63" spans="2:4">
       <c r="B63">
-        <v>59</v>
-      </c>
-      <c r="C63">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>2286</v>
+        <v>128</v>
       </c>
     </row>
     <row r="64" spans="2:4">
       <c r="B64">
-        <v>60</v>
-      </c>
-      <c r="C64">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>2287</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="2:4">
       <c r="B65">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>128</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="2:4">
       <c r="B66">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>148</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="2:4">
       <c r="B67">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>168</v>
+        <v>208</v>
       </c>
     </row>
     <row r="68" spans="2:4">
       <c r="B68">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>188</v>
+        <v>228</v>
       </c>
     </row>
     <row r="69" spans="2:4">
       <c r="B69">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>208</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="2:4">
       <c r="B70">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>228</v>
+        <v>268</v>
       </c>
     </row>
     <row r="71" spans="2:4">
       <c r="B71">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>248</v>
+        <v>288</v>
       </c>
     </row>
     <row r="72" spans="2:4">
       <c r="B72">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>268</v>
+        <v>308</v>
       </c>
     </row>
     <row r="73" spans="2:4">
       <c r="B73">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>288</v>
+        <v>328</v>
       </c>
     </row>
     <row r="74" spans="2:4">
       <c r="B74">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>308</v>
+        <v>348</v>
       </c>
     </row>
     <row r="75" spans="2:4">
       <c r="B75">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>328</v>
+        <v>368</v>
       </c>
     </row>
     <row r="76" spans="2:4">
       <c r="B76">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>348</v>
+        <v>388</v>
       </c>
     </row>
     <row r="77" spans="2:4">
       <c r="B77">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>368</v>
+        <v>408</v>
       </c>
     </row>
     <row r="78" spans="2:4">
       <c r="B78">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>388</v>
+        <v>428</v>
       </c>
     </row>
     <row r="79" spans="2:4">
       <c r="B79">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>408</v>
+        <v>448</v>
       </c>
     </row>
     <row r="80" spans="2:4">
       <c r="B80">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>428</v>
+        <v>468</v>
       </c>
     </row>
     <row r="81" spans="2:4">
       <c r="B81">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>448</v>
+        <v>488</v>
       </c>
     </row>
     <row r="82" spans="2:4">
       <c r="B82">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>468</v>
+        <v>508</v>
       </c>
     </row>
     <row r="83" spans="2:4">
       <c r="B83">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>488</v>
+        <v>528</v>
       </c>
     </row>
     <row r="84" spans="2:4">
       <c r="B84">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>508</v>
+        <v>548</v>
       </c>
     </row>
     <row r="85" spans="2:4">
       <c r="B85">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>528</v>
+        <v>568</v>
       </c>
     </row>
     <row r="86" spans="2:4">
       <c r="B86">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>548</v>
+        <v>588</v>
       </c>
     </row>
     <row r="87" spans="2:4">
       <c r="B87">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>568</v>
+        <v>608</v>
       </c>
     </row>
     <row r="88" spans="2:4">
       <c r="B88">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>588</v>
+        <v>628</v>
       </c>
     </row>
     <row r="89" spans="2:4">
       <c r="B89">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>608</v>
+        <v>648</v>
       </c>
     </row>
     <row r="90" spans="2:4">
       <c r="B90">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>628</v>
+        <v>668</v>
       </c>
     </row>
     <row r="91" spans="2:4">
       <c r="B91">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>648</v>
+        <v>688</v>
       </c>
     </row>
     <row r="92" spans="2:4">
       <c r="B92">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>668</v>
+        <v>708</v>
       </c>
     </row>
     <row r="93" spans="2:4">
       <c r="B93">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>688</v>
+        <v>728</v>
       </c>
     </row>
     <row r="94" spans="2:4">
       <c r="B94">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>708</v>
+        <v>748</v>
       </c>
     </row>
     <row r="95" spans="2:4">
       <c r="B95">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>728</v>
+        <v>768</v>
       </c>
     </row>
     <row r="96" spans="2:4">
       <c r="B96">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>748</v>
+        <v>788</v>
       </c>
     </row>
     <row r="97" spans="2:4">
       <c r="B97">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>768</v>
+        <v>808</v>
       </c>
     </row>
     <row r="98" spans="2:4">
       <c r="B98">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>788</v>
+        <v>828</v>
       </c>
     </row>
     <row r="99" spans="2:4">
       <c r="B99">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>808</v>
+        <v>848</v>
       </c>
     </row>
     <row r="100" spans="2:4">
       <c r="B100">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>828</v>
+        <v>868</v>
       </c>
     </row>
     <row r="101" spans="2:4">
       <c r="B101">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>848</v>
+        <v>888</v>
       </c>
     </row>
     <row r="102" spans="2:4">
       <c r="B102">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>868</v>
+        <v>908</v>
       </c>
     </row>
     <row r="103" spans="2:4">
       <c r="B103">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>888</v>
+        <v>928</v>
       </c>
     </row>
     <row r="104" spans="2:4">
       <c r="B104">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>908</v>
+        <v>948</v>
       </c>
     </row>
     <row r="105" spans="2:4">
       <c r="B105">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>928</v>
+        <v>968</v>
       </c>
     </row>
     <row r="106" spans="2:4">
       <c r="B106">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>948</v>
+        <v>988</v>
       </c>
     </row>
     <row r="107" spans="2:4">
       <c r="B107">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>968</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="108" spans="2:4">
       <c r="B108">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>988</v>
+        <v>1028</v>
       </c>
     </row>
     <row r="109" spans="2:4">
       <c r="B109">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>1008</v>
+        <v>1048</v>
       </c>
     </row>
     <row r="110" spans="2:4">
       <c r="B110">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>1028</v>
+        <v>1068</v>
       </c>
     </row>
     <row r="111" spans="2:4">
       <c r="B111">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>1048</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="112" spans="2:4">
       <c r="B112">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>1068</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="113" spans="2:4">
       <c r="B113">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>1088</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="114" spans="2:4">
       <c r="B114">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>1108</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="115" spans="2:4">
       <c r="B115">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>1128</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="116" spans="2:4">
       <c r="B116">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>1148</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="117" spans="2:4">
       <c r="B117">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1168</v>
+        <v>1208</v>
       </c>
     </row>
     <row r="118" spans="2:4">
       <c r="B118">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>1188</v>
+        <v>1228</v>
       </c>
     </row>
     <row r="119" spans="2:4">
       <c r="B119">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>1208</v>
+        <v>1248</v>
       </c>
     </row>
     <row r="120" spans="2:4">
       <c r="B120">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>1228</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="121" spans="2:4">
       <c r="B121">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>1248</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="122" spans="2:4">
       <c r="B122">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>1268</v>
+        <v>1308</v>
       </c>
     </row>
     <row r="123" spans="2:4">
       <c r="B123">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>1288</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="124" spans="2:4">
       <c r="B124">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>1308</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="125" spans="2:4">
       <c r="B125">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>1328</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="126" spans="2:4">
       <c r="B126">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>1348</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="127" spans="2:4">
       <c r="B127">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>1368</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="128" spans="2:4">
       <c r="B128">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>1388</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="129" spans="2:4">
       <c r="B129">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>1408</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="130" spans="2:4">
       <c r="B130">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="D130" s="1" t="s">
-        <v>1428</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="131" spans="2:4">
       <c r="B131">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>1448</v>
+        <v>1488</v>
       </c>
     </row>
     <row r="132" spans="2:4">
       <c r="B132">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>1468</v>
+        <v>1508</v>
       </c>
     </row>
     <row r="133" spans="2:4">
       <c r="B133">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>1488</v>
+        <v>1528</v>
       </c>
     </row>
     <row r="134" spans="2:4">
       <c r="B134">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>1508</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="135" spans="2:4">
       <c r="B135">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>1528</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="136" spans="2:4">
       <c r="B136">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>1548</v>
+        <v>1588</v>
       </c>
     </row>
     <row r="137" spans="2:4">
       <c r="B137">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>1568</v>
+        <v>1608</v>
       </c>
     </row>
     <row r="138" spans="2:4">
       <c r="B138">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>1588</v>
+        <v>1628</v>
       </c>
     </row>
     <row r="139" spans="2:4">
       <c r="B139">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>1608</v>
+        <v>1648</v>
       </c>
     </row>
     <row r="140" spans="2:4">
       <c r="B140">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1628</v>
+        <v>1668</v>
       </c>
     </row>
     <row r="141" spans="2:4">
       <c r="B141">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>1648</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="142" spans="2:4">
       <c r="B142">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>1668</v>
+        <v>1708</v>
       </c>
     </row>
     <row r="143" spans="2:4">
       <c r="B143">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>1688</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="144" spans="2:4">
       <c r="B144">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>1708</v>
+        <v>1748</v>
       </c>
     </row>
     <row r="145" spans="2:4">
       <c r="B145">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>1728</v>
+        <v>1768</v>
       </c>
     </row>
     <row r="146" spans="2:4">
       <c r="B146">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>1748</v>
+        <v>1788</v>
       </c>
     </row>
     <row r="147" spans="2:4">
       <c r="B147">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>1768</v>
+        <v>1808</v>
       </c>
     </row>
     <row r="148" spans="2:4">
       <c r="B148">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>1788</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="149" spans="2:4">
       <c r="B149">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>1808</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="150" spans="2:4">
       <c r="B150">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>1828</v>
+        <v>1868</v>
       </c>
     </row>
     <row r="151" spans="2:4">
       <c r="B151">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D151" s="1" t="s">
-        <v>1848</v>
+        <v>1888</v>
       </c>
     </row>
     <row r="152" spans="2:4">
       <c r="B152">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>1868</v>
+        <v>1908</v>
       </c>
     </row>
     <row r="153" spans="2:4">
       <c r="B153">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>1888</v>
+        <v>1928</v>
       </c>
     </row>
     <row r="154" spans="2:4">
       <c r="B154">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D154" s="1" t="s">
-        <v>1908</v>
+        <v>1948</v>
       </c>
     </row>
     <row r="155" spans="2:4">
       <c r="B155">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="D155" s="1" t="s">
-        <v>1928</v>
+        <v>1968</v>
       </c>
     </row>
     <row r="156" spans="2:4">
       <c r="B156">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D156" s="1" t="s">
-        <v>1948</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="157" spans="2:4">
       <c r="B157">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="D157" s="1" t="s">
-        <v>1968</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="158" spans="2:4">
       <c r="B158">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D158" s="1" t="s">
-        <v>1988</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="159" spans="2:4">
       <c r="B159">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="D159" s="1" t="s">
-        <v>2008</v>
+        <v>2048</v>
       </c>
     </row>
     <row r="160" spans="2:4">
       <c r="B160">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D160" s="1" t="s">
-        <v>2028</v>
+        <v>2068</v>
       </c>
     </row>
     <row r="161" spans="2:4">
       <c r="B161">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>2048</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="162" spans="2:4">
       <c r="B162">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D162" s="1" t="s">
-        <v>2068</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="163" spans="2:4">
       <c r="B163">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="D163" s="1" t="s">
-        <v>2088</v>
+        <v>143</v>
       </c>
     </row>
     <row r="164" spans="2:4">
       <c r="B164">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D164" s="1" t="s">
-        <v>2108</v>
+        <v>163</v>
       </c>
     </row>
     <row r="165" spans="2:4">
       <c r="B165">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="D165" s="1" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
     </row>
     <row r="166" spans="2:4">
       <c r="B166">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>163</v>
+        <v>203</v>
       </c>
     </row>
     <row r="167" spans="2:4">
       <c r="B167">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>183</v>
+        <v>223</v>
       </c>
     </row>
     <row r="168" spans="2:4">
       <c r="B168">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
     </row>
     <row r="169" spans="2:4">
       <c r="B169">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
     </row>
     <row r="170" spans="2:4">
       <c r="B170">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D170" s="1" t="s">
-        <v>243</v>
+        <v>283</v>
       </c>
     </row>
     <row r="171" spans="2:4">
       <c r="B171">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>263</v>
+        <v>303</v>
       </c>
     </row>
     <row r="172" spans="2:4">
       <c r="B172">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>283</v>
+        <v>323</v>
       </c>
     </row>
     <row r="173" spans="2:4">
       <c r="B173">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="D173" s="1" t="s">
-        <v>303</v>
+        <v>343</v>
       </c>
     </row>
     <row r="174" spans="2:4">
       <c r="B174">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="D174" s="1" t="s">
-        <v>323</v>
+        <v>363</v>
       </c>
     </row>
     <row r="175" spans="2:4">
       <c r="B175">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D175" s="1" t="s">
-        <v>343</v>
+        <v>383</v>
       </c>
     </row>
     <row r="176" spans="2:4">
       <c r="B176">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="D176" s="1" t="s">
-        <v>363</v>
+        <v>403</v>
       </c>
     </row>
     <row r="177" spans="2:4">
       <c r="B177">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="D177" s="1" t="s">
-        <v>383</v>
+        <v>423</v>
       </c>
     </row>
     <row r="178" spans="2:4">
       <c r="B178">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="D178" s="1" t="s">
-        <v>403</v>
+        <v>443</v>
       </c>
     </row>
     <row r="179" spans="2:4">
       <c r="B179">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D179" s="1" t="s">
-        <v>423</v>
+        <v>463</v>
       </c>
     </row>
     <row r="180" spans="2:4">
       <c r="B180">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="D180" s="1" t="s">
-        <v>443</v>
+        <v>483</v>
       </c>
     </row>
     <row r="181" spans="2:4">
       <c r="B181">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="D181" s="1" t="s">
-        <v>463</v>
+        <v>503</v>
       </c>
     </row>
     <row r="182" spans="2:4">
       <c r="B182">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="D182" s="1" t="s">
-        <v>483</v>
+        <v>523</v>
       </c>
     </row>
     <row r="183" spans="2:4">
       <c r="B183">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>503</v>
+        <v>543</v>
       </c>
     </row>
     <row r="184" spans="2:4">
       <c r="B184">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D184" s="1" t="s">
-        <v>523</v>
+        <v>563</v>
       </c>
     </row>
     <row r="185" spans="2:4">
       <c r="B185">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="D185" s="1" t="s">
-        <v>543</v>
+        <v>583</v>
       </c>
     </row>
     <row r="186" spans="2:4">
       <c r="B186">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="D186" s="1" t="s">
-        <v>563</v>
+        <v>603</v>
       </c>
     </row>
     <row r="187" spans="2:4">
       <c r="B187">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="D187" s="1" t="s">
-        <v>583</v>
+        <v>623</v>
       </c>
     </row>
     <row r="188" spans="2:4">
       <c r="B188">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>603</v>
+        <v>643</v>
       </c>
     </row>
     <row r="189" spans="2:4">
       <c r="B189">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D189" s="1" t="s">
-        <v>623</v>
+        <v>663</v>
       </c>
     </row>
     <row r="190" spans="2:4">
       <c r="B190">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="D190" s="1" t="s">
-        <v>643</v>
+        <v>683</v>
       </c>
     </row>
     <row r="191" spans="2:4">
       <c r="B191">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D191" s="1" t="s">
-        <v>663</v>
+        <v>703</v>
       </c>
     </row>
     <row r="192" spans="2:4">
       <c r="B192">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D192" s="1" t="s">
-        <v>683</v>
+        <v>723</v>
       </c>
     </row>
     <row r="193" spans="2:4">
       <c r="B193">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="D193" s="1" t="s">
-        <v>703</v>
+        <v>743</v>
       </c>
     </row>
     <row r="194" spans="2:4">
       <c r="B194">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="D194" s="1" t="s">
-        <v>723</v>
+        <v>763</v>
       </c>
     </row>
     <row r="195" spans="2:4">
       <c r="B195">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="D195" s="1" t="s">
-        <v>743</v>
+        <v>783</v>
       </c>
     </row>
     <row r="196" spans="2:4">
       <c r="B196">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="D196" s="1" t="s">
-        <v>763</v>
+        <v>803</v>
       </c>
     </row>
     <row r="197" spans="2:4">
       <c r="B197">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>783</v>
+        <v>823</v>
       </c>
     </row>
     <row r="198" spans="2:4">
       <c r="B198">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D198" s="1" t="s">
-        <v>803</v>
+        <v>843</v>
       </c>
     </row>
     <row r="199" spans="2:4">
       <c r="B199">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="D199" s="1" t="s">
-        <v>823</v>
+        <v>863</v>
       </c>
     </row>
     <row r="200" spans="2:4">
       <c r="B200">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D200" s="1" t="s">
-        <v>843</v>
+        <v>883</v>
       </c>
     </row>
     <row r="201" spans="2:4">
       <c r="B201">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="D201" s="1" t="s">
-        <v>863</v>
+        <v>903</v>
       </c>
     </row>
     <row r="202" spans="2:4">
       <c r="B202">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="D202" s="1" t="s">
-        <v>883</v>
+        <v>923</v>
       </c>
     </row>
     <row r="203" spans="2:4">
       <c r="B203">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="D203" s="1" t="s">
-        <v>903</v>
+        <v>943</v>
       </c>
     </row>
     <row r="204" spans="2:4">
       <c r="B204">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="D204" s="1" t="s">
-        <v>923</v>
+        <v>963</v>
       </c>
     </row>
     <row r="205" spans="2:4">
       <c r="B205">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="D205" s="1" t="s">
-        <v>943</v>
+        <v>983</v>
       </c>
     </row>
     <row r="206" spans="2:4">
       <c r="B206">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>963</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="207" spans="2:4">
       <c r="B207">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="D207" s="1" t="s">
-        <v>983</v>
+        <v>1023</v>
       </c>
     </row>
     <row r="208" spans="2:4">
       <c r="B208">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>1003</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="209" spans="2:4">
       <c r="B209">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="D209" s="1" t="s">
-        <v>1023</v>
+        <v>1063</v>
       </c>
     </row>
     <row r="210" spans="2:4">
       <c r="B210">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D210" s="1" t="s">
-        <v>1043</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="211" spans="2:4">
       <c r="B211">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>1063</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="212" spans="2:4">
       <c r="B212">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D212" s="1" t="s">
-        <v>1083</v>
+        <v>1123</v>
       </c>
     </row>
     <row r="213" spans="2:4">
       <c r="B213">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>1103</v>
+        <v>1143</v>
       </c>
     </row>
     <row r="214" spans="2:4">
       <c r="B214">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D214" s="1" t="s">
-        <v>1123</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="215" spans="2:4">
       <c r="B215">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="D215" s="1" t="s">
-        <v>1143</v>
+        <v>1183</v>
       </c>
     </row>
     <row r="216" spans="2:4">
       <c r="B216">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>1163</v>
+        <v>1203</v>
       </c>
     </row>
     <row r="217" spans="2:4">
       <c r="B217">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1183</v>
+        <v>1223</v>
       </c>
     </row>
     <row r="218" spans="2:4">
       <c r="B218">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D218" s="1" t="s">
-        <v>1203</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="219" spans="2:4">
       <c r="B219">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D219" s="1" t="s">
-        <v>1223</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="220" spans="2:4">
       <c r="B220">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D220" s="1" t="s">
-        <v>1243</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="221" spans="2:4">
       <c r="B221">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D221" s="1" t="s">
-        <v>1263</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="222" spans="2:4">
       <c r="B222">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="D222" s="1" t="s">
-        <v>1283</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="223" spans="2:4">
       <c r="B223">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D223" s="1" t="s">
-        <v>1303</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="224" spans="2:4">
       <c r="B224">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D224" s="1" t="s">
-        <v>1323</v>
+        <v>1363</v>
       </c>
     </row>
     <row r="225" spans="2:4">
       <c r="B225">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D225" s="1" t="s">
-        <v>1343</v>
+        <v>1383</v>
       </c>
     </row>
     <row r="226" spans="2:4">
       <c r="B226">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="D226" s="1" t="s">
-        <v>1363</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="227" spans="2:4">
       <c r="B227">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D227" s="1" t="s">
-        <v>1383</v>
+        <v>1423</v>
       </c>
     </row>
     <row r="228" spans="2:4">
       <c r="B228">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="D228" s="1" t="s">
-        <v>1403</v>
+        <v>1443</v>
       </c>
     </row>
     <row r="229" spans="2:4">
       <c r="B229">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="D229" s="1" t="s">
-        <v>1423</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="230" spans="2:4">
       <c r="B230">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="D230" s="1" t="s">
-        <v>1443</v>
+        <v>1483</v>
       </c>
     </row>
     <row r="231" spans="2:4">
       <c r="B231">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="D231" s="1" t="s">
-        <v>1463</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="232" spans="2:4">
       <c r="B232">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="D232" s="1" t="s">
-        <v>1483</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="233" spans="2:4">
       <c r="B233">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="D233" s="1" t="s">
-        <v>1503</v>
+        <v>1543</v>
       </c>
     </row>
     <row r="234" spans="2:4">
       <c r="B234">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>1523</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="235" spans="2:4">
       <c r="B235">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="D235" s="1" t="s">
-        <v>1543</v>
+        <v>1583</v>
       </c>
     </row>
     <row r="236" spans="2:4">
       <c r="B236">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D236" s="1" t="s">
-        <v>1563</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="237" spans="2:4">
       <c r="B237">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>1583</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="238" spans="2:4">
       <c r="B238">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="D238" s="1" t="s">
-        <v>1603</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="239" spans="2:4">
       <c r="B239">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="D239" s="1" t="s">
-        <v>1623</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="240" spans="2:4">
       <c r="B240">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="D240" s="1" t="s">
-        <v>1643</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="241" spans="2:4">
       <c r="B241">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="D241" s="1" t="s">
-        <v>1663</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="242" spans="2:4">
       <c r="B242">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="D242" s="1" t="s">
-        <v>1683</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="243" spans="2:4">
       <c r="B243">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1703</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="244" spans="2:4">
       <c r="B244">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="D244" s="1" t="s">
-        <v>1723</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="245" spans="2:4">
       <c r="B245">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="D245" s="1" t="s">
-        <v>1743</v>
+        <v>1783</v>
       </c>
     </row>
     <row r="246" spans="2:4">
       <c r="B246">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="D246" s="1" t="s">
-        <v>1763</v>
+        <v>1803</v>
       </c>
     </row>
     <row r="247" spans="2:4">
       <c r="B247">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="D247" s="1" t="s">
-        <v>1783</v>
+        <v>1823</v>
       </c>
     </row>
     <row r="248" spans="2:4">
       <c r="B248">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="D248" s="1" t="s">
-        <v>1803</v>
+        <v>1843</v>
       </c>
     </row>
     <row r="249" spans="2:4">
       <c r="B249">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D249" s="1" t="s">
-        <v>1823</v>
+        <v>1863</v>
       </c>
     </row>
     <row r="250" spans="2:4">
       <c r="B250">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>1843</v>
+        <v>1883</v>
       </c>
     </row>
     <row r="251" spans="2:4">
       <c r="B251">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D251" s="1" t="s">
-        <v>1863</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="252" spans="2:4">
       <c r="B252">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D252" s="1" t="s">
-        <v>1883</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="253" spans="2:4">
       <c r="B253">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="D253" s="1" t="s">
-        <v>1903</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="254" spans="2:4">
       <c r="B254">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="D254" s="1" t="s">
-        <v>1923</v>
+        <v>1963</v>
       </c>
     </row>
     <row r="255" spans="2:4">
       <c r="B255">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>1943</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="256" spans="2:4">
       <c r="B256">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D256" s="1" t="s">
-        <v>1963</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="257" spans="2:4">
       <c r="B257">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="D257" s="1" t="s">
-        <v>1983</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="258" spans="2:4">
       <c r="B258">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D258" s="1" t="s">
-        <v>2003</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="259" spans="2:4">
       <c r="B259">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="D259" s="1" t="s">
-        <v>2023</v>
+        <v>2063</v>
       </c>
     </row>
     <row r="260" spans="2:4">
       <c r="B260">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D260" s="1" t="s">
-        <v>2043</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="261" spans="2:4">
       <c r="B261">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="D261" s="1" t="s">
-        <v>2063</v>
+        <v>2103</v>
       </c>
     </row>
     <row r="262" spans="2:4">
       <c r="B262">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="D262" s="1" t="s">
-        <v>2083</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="263" spans="2:4">
       <c r="B263">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D263" s="1" t="s">
-        <v>2103</v>
+        <v>138</v>
       </c>
     </row>
     <row r="264" spans="2:4">
       <c r="B264">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="D264" s="1" t="s">
-        <v>2123</v>
+        <v>158</v>
       </c>
     </row>
     <row r="265" spans="2:4">
       <c r="B265">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D265" s="1" t="s">
-        <v>138</v>
+        <v>178</v>
       </c>
     </row>
     <row r="266" spans="2:4">
       <c r="B266">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="D266" s="1" t="s">
-        <v>158</v>
+        <v>198</v>
       </c>
     </row>
     <row r="267" spans="2:4">
       <c r="B267">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D267" s="1" t="s">
-        <v>178</v>
+        <v>218</v>
       </c>
     </row>
     <row r="268" spans="2:4">
       <c r="B268">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="D268" s="1" t="s">
-        <v>198</v>
+        <v>238</v>
       </c>
     </row>
     <row r="269" spans="2:4">
       <c r="B269">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D269" s="1" t="s">
-        <v>218</v>
+        <v>258</v>
       </c>
     </row>
     <row r="270" spans="2:4">
       <c r="B270">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>238</v>
+        <v>278</v>
       </c>
     </row>
     <row r="271" spans="2:4">
       <c r="B271">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>258</v>
+        <v>298</v>
       </c>
     </row>
     <row r="272" spans="2:4">
       <c r="B272">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="D272" s="1" t="s">
-        <v>278</v>
+        <v>318</v>
       </c>
     </row>
     <row r="273" spans="2:4">
       <c r="B273">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="D273" s="1" t="s">
-        <v>298</v>
+        <v>338</v>
       </c>
     </row>
     <row r="274" spans="2:4">
       <c r="B274">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="D274" s="1" t="s">
-        <v>318</v>
+        <v>358</v>
       </c>
     </row>
     <row r="275" spans="2:4">
       <c r="B275">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>338</v>
+        <v>378</v>
       </c>
     </row>
     <row r="276" spans="2:4">
       <c r="B276">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="D276" s="1" t="s">
-        <v>358</v>
+        <v>398</v>
       </c>
     </row>
     <row r="277" spans="2:4">
       <c r="B277">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="D277" s="1" t="s">
-        <v>378</v>
+        <v>418</v>
       </c>
     </row>
     <row r="278" spans="2:4">
       <c r="B278">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D278" s="1" t="s">
-        <v>398</v>
+        <v>438</v>
       </c>
     </row>
     <row r="279" spans="2:4">
       <c r="B279">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="D279" s="1" t="s">
-        <v>418</v>
+        <v>458</v>
       </c>
     </row>
     <row r="280" spans="2:4">
       <c r="B280">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D280" s="1" t="s">
-        <v>438</v>
+        <v>478</v>
       </c>
     </row>
     <row r="281" spans="2:4">
       <c r="B281">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="D281" s="1" t="s">
-        <v>458</v>
+        <v>498</v>
       </c>
     </row>
     <row r="282" spans="2:4">
       <c r="B282">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D282" s="1" t="s">
-        <v>478</v>
+        <v>518</v>
       </c>
     </row>
     <row r="283" spans="2:4">
       <c r="B283">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="D283" s="1" t="s">
-        <v>498</v>
+        <v>538</v>
       </c>
     </row>
     <row r="284" spans="2:4">
       <c r="B284">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>518</v>
+        <v>558</v>
       </c>
     </row>
     <row r="285" spans="2:4">
       <c r="B285">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D285" s="1" t="s">
-        <v>538</v>
+        <v>578</v>
       </c>
     </row>
     <row r="286" spans="2:4">
       <c r="B286">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="D286" s="1" t="s">
-        <v>558</v>
+        <v>598</v>
       </c>
     </row>
     <row r="287" spans="2:4">
       <c r="B287">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="D287" s="1" t="s">
-        <v>578</v>
+        <v>618</v>
       </c>
     </row>
     <row r="288" spans="2:4">
       <c r="B288">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>598</v>
+        <v>638</v>
       </c>
     </row>
     <row r="289" spans="2:4">
       <c r="B289">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="D289" s="1" t="s">
-        <v>618</v>
+        <v>658</v>
       </c>
     </row>
     <row r="290" spans="2:4">
       <c r="B290">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>638</v>
+        <v>678</v>
       </c>
     </row>
     <row r="291" spans="2:4">
       <c r="B291">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>658</v>
+        <v>698</v>
       </c>
     </row>
     <row r="292" spans="2:4">
       <c r="B292">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>678</v>
+        <v>718</v>
       </c>
     </row>
     <row r="293" spans="2:4">
       <c r="B293">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="D293" s="1" t="s">
-        <v>698</v>
+        <v>738</v>
       </c>
     </row>
     <row r="294" spans="2:4">
       <c r="B294">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="D294" s="1" t="s">
-        <v>718</v>
+        <v>758</v>
       </c>
     </row>
     <row r="295" spans="2:4">
       <c r="B295">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="D295" s="1" t="s">
-        <v>738</v>
+        <v>778</v>
       </c>
     </row>
     <row r="296" spans="2:4">
       <c r="B296">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="D296" s="1" t="s">
-        <v>758</v>
+        <v>798</v>
       </c>
     </row>
     <row r="297" spans="2:4">
       <c r="B297">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D297" s="1" t="s">
-        <v>778</v>
+        <v>818</v>
       </c>
     </row>
     <row r="298" spans="2:4">
       <c r="B298">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="D298" s="1" t="s">
-        <v>798</v>
+        <v>838</v>
       </c>
     </row>
     <row r="299" spans="2:4">
       <c r="B299">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="D299" s="1" t="s">
-        <v>818</v>
+        <v>858</v>
       </c>
     </row>
     <row r="300" spans="2:4">
       <c r="B300">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="D300" s="1" t="s">
-        <v>838</v>
+        <v>878</v>
       </c>
     </row>
     <row r="301" spans="2:4">
       <c r="B301">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="D301" s="1" t="s">
-        <v>858</v>
+        <v>898</v>
       </c>
     </row>
     <row r="302" spans="2:4">
       <c r="B302">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>878</v>
+        <v>918</v>
       </c>
     </row>
     <row r="303" spans="2:4">
       <c r="B303">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="D303" s="1" t="s">
-        <v>898</v>
+        <v>938</v>
       </c>
     </row>
     <row r="304" spans="2:4">
       <c r="B304">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="D304" s="1" t="s">
-        <v>918</v>
+        <v>958</v>
       </c>
     </row>
     <row r="305" spans="2:4">
       <c r="B305">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>938</v>
+        <v>978</v>
       </c>
     </row>
     <row r="306" spans="2:4">
       <c r="B306">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="D306" s="1" t="s">
-        <v>958</v>
+        <v>998</v>
       </c>
     </row>
     <row r="307" spans="2:4">
       <c r="B307">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="D307" s="1" t="s">
-        <v>978</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="308" spans="2:4">
       <c r="B308">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="D308" s="1" t="s">
-        <v>998</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="309" spans="2:4">
       <c r="B309">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="D309" s="1" t="s">
-        <v>1018</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="310" spans="2:4">
       <c r="B310">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="D310" s="1" t="s">
-        <v>1038</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="311" spans="2:4">
       <c r="B311">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="D311" s="1" t="s">
-        <v>1058</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="312" spans="2:4">
       <c r="B312">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>1078</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="313" spans="2:4">
       <c r="B313">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>1098</v>
+        <v>1138</v>
       </c>
     </row>
     <row r="314" spans="2:4">
       <c r="B314">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="D314" s="1" t="s">
-        <v>1118</v>
+        <v>1158</v>
       </c>
     </row>
     <row r="315" spans="2:4">
       <c r="B315">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="D315" s="1" t="s">
-        <v>1138</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="316" spans="2:4">
       <c r="B316">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="D316" s="1" t="s">
-        <v>1158</v>
+        <v>1198</v>
       </c>
     </row>
     <row r="317" spans="2:4">
       <c r="B317">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="D317" s="1" t="s">
-        <v>1178</v>
+        <v>1218</v>
       </c>
     </row>
     <row r="318" spans="2:4">
       <c r="B318">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="D318" s="1" t="s">
-        <v>1198</v>
+        <v>1238</v>
       </c>
     </row>
     <row r="319" spans="2:4">
       <c r="B319">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="D319" s="1" t="s">
-        <v>1218</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="320" spans="2:4">
       <c r="B320">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>1238</v>
+        <v>1278</v>
       </c>
     </row>
     <row r="321" spans="2:4">
       <c r="B321">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="D321" s="1" t="s">
-        <v>1258</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="322" spans="2:4">
       <c r="B322">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D322" s="1" t="s">
-        <v>1278</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="323" spans="2:4">
       <c r="B323">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="D323" s="1" t="s">
-        <v>1298</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="324" spans="2:4">
       <c r="B324">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>1318</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="325" spans="2:4">
       <c r="B325">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="D325" s="1" t="s">
-        <v>1338</v>
+        <v>1378</v>
       </c>
     </row>
     <row r="326" spans="2:4">
       <c r="B326">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="D326" s="1" t="s">
-        <v>1358</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="327" spans="2:4">
       <c r="B327">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>1378</v>
+        <v>1418</v>
       </c>
     </row>
     <row r="328" spans="2:4">
       <c r="B328">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="D328" s="1" t="s">
-        <v>1398</v>
+        <v>1438</v>
       </c>
     </row>
     <row r="329" spans="2:4">
       <c r="B329">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="D329" s="1" t="s">
-        <v>1418</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="330" spans="2:4">
       <c r="B330">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="D330" s="1" t="s">
-        <v>1438</v>
+        <v>1478</v>
       </c>
     </row>
     <row r="331" spans="2:4">
       <c r="B331">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="D331" s="1" t="s">
-        <v>1458</v>
+        <v>1498</v>
       </c>
     </row>
     <row r="332" spans="2:4">
       <c r="B332">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D332" s="1" t="s">
-        <v>1478</v>
+        <v>1518</v>
       </c>
     </row>
     <row r="333" spans="2:4">
       <c r="B333">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="D333" s="1" t="s">
-        <v>1498</v>
+        <v>1538</v>
       </c>
     </row>
     <row r="334" spans="2:4">
       <c r="B334">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="D334" s="1" t="s">
-        <v>1518</v>
+        <v>1558</v>
       </c>
     </row>
     <row r="335" spans="2:4">
       <c r="B335">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="D335" s="1" t="s">
-        <v>1538</v>
+        <v>1578</v>
       </c>
     </row>
     <row r="336" spans="2:4">
       <c r="B336">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="D336" s="1" t="s">
-        <v>1558</v>
+        <v>1598</v>
       </c>
     </row>
     <row r="337" spans="2:4">
       <c r="B337">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="D337" s="1" t="s">
-        <v>1578</v>
+        <v>1618</v>
       </c>
     </row>
     <row r="338" spans="2:4">
       <c r="B338">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D338" s="1" t="s">
-        <v>1598</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="339" spans="2:4">
       <c r="B339">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="D339" s="1" t="s">
-        <v>1618</v>
+        <v>1658</v>
       </c>
     </row>
     <row r="340" spans="2:4">
       <c r="B340">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="D340" s="1" t="s">
-        <v>1638</v>
+        <v>1678</v>
       </c>
     </row>
     <row r="341" spans="2:4">
       <c r="B341">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="D341" s="1" t="s">
-        <v>1658</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="342" spans="2:4">
       <c r="B342">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="D342" s="1" t="s">
-        <v>1678</v>
+        <v>1718</v>
       </c>
     </row>
     <row r="343" spans="2:4">
       <c r="B343">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="D343" s="1" t="s">
-        <v>1698</v>
+        <v>1738</v>
       </c>
     </row>
     <row r="344" spans="2:4">
       <c r="B344">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="D344" s="1" t="s">
-        <v>1718</v>
+        <v>1758</v>
       </c>
     </row>
     <row r="345" spans="2:4">
       <c r="B345">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="D345" s="1" t="s">
-        <v>1738</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="346" spans="2:4">
       <c r="B346">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="D346" s="1" t="s">
-        <v>1758</v>
+        <v>1798</v>
       </c>
     </row>
     <row r="347" spans="2:4">
       <c r="B347">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="D347" s="1" t="s">
-        <v>1778</v>
+        <v>1818</v>
       </c>
     </row>
     <row r="348" spans="2:4">
       <c r="B348">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D348" s="1" t="s">
-        <v>1798</v>
+        <v>1838</v>
       </c>
     </row>
     <row r="349" spans="2:4">
       <c r="B349">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="D349" s="1" t="s">
-        <v>1818</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="350" spans="2:4">
       <c r="B350">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="D350" s="1" t="s">
-        <v>1838</v>
+        <v>1878</v>
       </c>
     </row>
     <row r="351" spans="2:4">
       <c r="B351">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="D351" s="1" t="s">
-        <v>1858</v>
+        <v>1898</v>
       </c>
     </row>
     <row r="352" spans="2:4">
       <c r="B352">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="D352" s="1" t="s">
-        <v>1878</v>
+        <v>1918</v>
       </c>
     </row>
     <row r="353" spans="2:4">
       <c r="B353">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="D353" s="1" t="s">
-        <v>1898</v>
+        <v>1938</v>
       </c>
     </row>
     <row r="354" spans="2:4">
       <c r="B354">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="D354" s="1" t="s">
-        <v>1918</v>
+        <v>1958</v>
       </c>
     </row>
     <row r="355" spans="2:4">
       <c r="B355">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="D355" s="1" t="s">
-        <v>1938</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="356" spans="2:4">
       <c r="B356">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="D356" s="1" t="s">
-        <v>1958</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="357" spans="2:4">
       <c r="B357">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="D357" s="1" t="s">
-        <v>1978</v>
+        <v>2018</v>
       </c>
     </row>
     <row r="358" spans="2:4">
       <c r="B358">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="D358" s="1" t="s">
-        <v>1998</v>
+        <v>2038</v>
       </c>
     </row>
     <row r="359" spans="2:4">
       <c r="B359">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="D359" s="1" t="s">
-        <v>2018</v>
+        <v>2058</v>
       </c>
     </row>
     <row r="360" spans="2:4">
       <c r="B360">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="D360" s="1" t="s">
-        <v>2038</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="361" spans="2:4">
       <c r="B361">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="D361" s="1" t="s">
-        <v>2058</v>
+        <v>2098</v>
       </c>
     </row>
     <row r="362" spans="2:4">
       <c r="B362">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>2078</v>
-      </c>
-    </row>
-    <row r="363" spans="2:4">
-      <c r="B363">
-        <v>359</v>
-      </c>
-      <c r="D363" s="1" t="s">
-        <v>2098</v>
-      </c>
-    </row>
-    <row r="364" spans="2:4">
-      <c r="B364">
-        <v>360</v>
-      </c>
-      <c r="D364" s="1" t="s">
         <v>2118</v>
+      </c>
+    </row>
+    <row r="366" spans="2:4">
+      <c r="B366">
+        <f>36.794652</f>
+        <v>36.794651999999999</v>
+      </c>
+    </row>
+    <row r="367" spans="2:4">
+      <c r="B367">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="368" spans="2:4">
+      <c r="B368">
+        <f>47/60</f>
+        <v>0.78333333333333333</v>
+      </c>
+    </row>
+    <row r="369" spans="2:2">
+      <c r="B369">
+        <f>B366-B367-B368</f>
+        <v>1.1318666666665922E-2</v>
+      </c>
+    </row>
+    <row r="370" spans="2:2">
+      <c r="B370">
+        <f>B369*3600</f>
+        <v>40.747199999997321</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added picture upload(carrierwave),edit,and delete capabilities for user and for community
</commit_message>
<xml_diff>
--- a/Seed_Table_for_Address_Names.xlsx
+++ b/Seed_Table_for_Address_Names.xlsx
@@ -7341,14 +7341,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D370"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A344" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="B371" sqref="B371"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="2" max="2" width="12.83203125" customWidth="1"/>
-    <col min="3" max="3" width="16.83203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="16.83203125" customWidth="1"/>
     <col min="4" max="4" width="15.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -10481,8 +10481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C5:W105"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6:N105"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17155,7 +17155,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="str">
-        <f t="shared" ref="C7:I25" si="2">CONCATENATE(C$5,$B7)</f>
+        <f t="shared" ref="C7:G25" si="2">CONCATENATE(C$5,$B7)</f>
         <v>ac</v>
       </c>
       <c r="D7" t="str">

</xml_diff>